<commit_message>
Update leapsec function | Update docs.
</commit_message>
<xml_diff>
--- a/src/maser_tools/maser/tools/support/cdf/converter_example.xlsx
+++ b/src/maser_tools/maser/tools/support/cdf/converter_example.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10911"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xbonnin/Work/Projects/MASER/Software/Git/maser4py/src/maser_tools/maser/tools/support/cdf/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD5DF2E-9B82-8640-8551-3BA2B81B07C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27360" yWindow="-80" windowWidth="25360" windowHeight="15820" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20440" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="header" sheetId="1" r:id="rId1"/>
@@ -14,7 +20,7 @@
     <sheet name="Options" sheetId="5" r:id="rId5"/>
     <sheet name="NRV" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="120">
   <si>
     <t>CDF NAME</t>
   </si>
@@ -369,12 +375,27 @@
   </si>
   <si>
     <t>DEPEND_0</t>
+  </si>
+  <si>
+    <t>VAR_SPARESERECORDS</t>
+  </si>
+  <si>
+    <t>GZIP.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0000-01-01T00:00:00.000000000</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>" "</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -749,7 +770,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -804,6 +825,9 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="279">
@@ -1089,6 +1113,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1413,14 +1445,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="47.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
@@ -1430,7 +1462,7 @@
     <col min="6" max="6" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1443,8 +1475,14 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>106</v>
       </c>
@@ -1456,6 +1494,12 @@
       </c>
       <c r="D2" t="s">
         <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1470,14 +1514,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
@@ -1485,7 +1529,7 @@
     <col min="4" max="4" width="108.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1499,7 +1543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1513,7 +1557,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1527,7 +1571,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1541,7 +1585,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1555,7 +1599,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1569,7 +1613,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1583,7 +1627,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1594,7 +1638,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1608,7 +1652,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1622,7 +1666,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -1636,7 +1680,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1650,7 +1694,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -1664,7 +1708,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1678,7 +1722,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -1692,7 +1736,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1706,7 +1750,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -1720,7 +1764,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -1731,7 +1775,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1742,7 +1786,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -1756,7 +1800,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -1782,14 +1826,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.1640625" style="4" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
@@ -1798,11 +1842,11 @@
     <col min="6" max="6" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.33203125" customWidth="1"/>
+    <col min="10" max="10" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -1824,8 +1868,17 @@
       <c r="G1" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="H1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>58</v>
       </c>
@@ -1841,11 +1894,14 @@
       <c r="F2" t="s">
         <v>38</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="H2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>80</v>
       </c>
@@ -1867,11 +1923,15 @@
       <c r="G3" t="s">
         <v>38</v>
       </c>
-      <c r="H3" s="1"/>
+      <c r="H3" t="s">
+        <v>116</v>
+      </c>
       <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="J3" s="27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>81</v>
       </c>
@@ -1893,11 +1953,15 @@
       <c r="G4" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H4" s="1"/>
+      <c r="H4" t="s">
+        <v>41</v>
+      </c>
       <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="J4" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>85</v>
       </c>
@@ -1919,9 +1983,13 @@
       <c r="G5" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="1"/>
+      <c r="H5" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>119</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1935,14 +2003,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D686"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="33.1640625" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
@@ -1950,7 +2018,7 @@
     <col min="4" max="4" width="68.83203125" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -1964,7 +2032,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -1978,7 +2046,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -1992,7 +2060,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -2006,7 +2074,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -2020,7 +2088,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -2034,7 +2102,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -2048,7 +2116,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>58</v>
       </c>
@@ -2062,7 +2130,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -2076,7 +2144,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>58</v>
       </c>
@@ -2090,7 +2158,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -2104,7 +2172,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -2118,7 +2186,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -2132,7 +2200,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>58</v>
       </c>
@@ -2146,7 +2214,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>58</v>
       </c>
@@ -2160,7 +2228,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -2174,7 +2242,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -2188,7 +2256,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -2200,7 +2268,7 @@
       </c>
       <c r="D18" s="25"/>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>80</v>
       </c>
@@ -2214,7 +2282,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>80</v>
       </c>
@@ -2228,7 +2296,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="14" t="s">
         <v>80</v>
       </c>
@@ -2242,7 +2310,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
         <v>80</v>
       </c>
@@ -2256,7 +2324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>80</v>
       </c>
@@ -2270,7 +2338,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="14" t="s">
         <v>80</v>
       </c>
@@ -2284,7 +2352,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="14" t="s">
         <v>80</v>
       </c>
@@ -2298,7 +2366,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
         <v>80</v>
       </c>
@@ -2312,7 +2380,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
         <v>80</v>
       </c>
@@ -2326,7 +2394,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
         <v>80</v>
       </c>
@@ -2340,7 +2408,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>80</v>
       </c>
@@ -2354,7 +2422,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="14" customFormat="1">
+    <row r="30" spans="1:4" s="14" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
         <v>81</v>
       </c>
@@ -2368,7 +2436,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="14" t="s">
         <v>81</v>
       </c>
@@ -2382,7 +2450,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>81</v>
       </c>
@@ -2396,7 +2464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
         <v>81</v>
       </c>
@@ -2410,7 +2478,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="14" t="s">
         <v>81</v>
       </c>
@@ -2424,7 +2492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="14" t="s">
         <v>81</v>
       </c>
@@ -2438,7 +2506,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>81</v>
       </c>
@@ -2452,7 +2520,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="14" t="s">
         <v>81</v>
       </c>
@@ -2466,7 +2534,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="14" t="s">
         <v>81</v>
       </c>
@@ -2480,7 +2548,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="14" t="s">
         <v>85</v>
       </c>
@@ -2494,7 +2562,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="16" t="s">
         <v>85</v>
       </c>
@@ -2508,2796 +2576,2796 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:4" s="14" customFormat="1">
+    <row r="42" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42"/>
       <c r="B42"/>
       <c r="C42"/>
       <c r="D42" s="10"/>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="11"/>
       <c r="B59" s="12"/>
       <c r="C59" s="11"/>
       <c r="D59" s="13"/>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="14"/>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="14"/>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="14"/>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="14"/>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="14"/>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="14"/>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" s="14"/>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="14"/>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" s="14"/>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="14"/>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="14"/>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="14"/>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="14"/>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="14"/>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="14"/>
     </row>
-    <row r="75" spans="1:4">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" s="11"/>
       <c r="B75" s="12"/>
       <c r="C75" s="11"/>
       <c r="D75" s="13"/>
     </row>
-    <row r="76" spans="1:4">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" s="14"/>
     </row>
-    <row r="77" spans="1:4">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="14"/>
     </row>
-    <row r="78" spans="1:4">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" s="14"/>
     </row>
-    <row r="79" spans="1:4">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" s="14"/>
     </row>
-    <row r="80" spans="1:4">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" s="14"/>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" s="14"/>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" s="14"/>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" s="14"/>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" s="14"/>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="14"/>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="14"/>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="14"/>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="14"/>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="14"/>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="14"/>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="14"/>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="16"/>
     </row>
-    <row r="93" spans="1:4">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="12"/>
       <c r="B93" s="12"/>
       <c r="C93" s="11"/>
       <c r="D93" s="13"/>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="4"/>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="4"/>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="4"/>
     </row>
-    <row r="97" spans="1:4">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="4"/>
     </row>
-    <row r="98" spans="1:4">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="4"/>
     </row>
-    <row r="99" spans="1:4">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A99" s="4"/>
     </row>
-    <row r="100" spans="1:4">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="4"/>
     </row>
-    <row r="101" spans="1:4">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="4"/>
     </row>
-    <row r="102" spans="1:4">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="4"/>
     </row>
-    <row r="103" spans="1:4">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="4"/>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="4"/>
     </row>
-    <row r="105" spans="1:4">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="4"/>
     </row>
-    <row r="106" spans="1:4">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="4"/>
     </row>
-    <row r="107" spans="1:4">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="4"/>
     </row>
-    <row r="108" spans="1:4">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A108" s="4"/>
     </row>
-    <row r="109" spans="1:4">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A109" s="4"/>
     </row>
-    <row r="110" spans="1:4">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="4"/>
     </row>
-    <row r="111" spans="1:4">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="12"/>
       <c r="B111" s="12"/>
       <c r="C111" s="11"/>
       <c r="D111" s="13"/>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A112" s="4"/>
     </row>
-    <row r="113" spans="1:1">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" s="4"/>
     </row>
-    <row r="114" spans="1:1">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" s="4"/>
     </row>
-    <row r="115" spans="1:1">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" s="4"/>
     </row>
-    <row r="116" spans="1:1">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" s="4"/>
     </row>
-    <row r="117" spans="1:1">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" s="4"/>
     </row>
-    <row r="118" spans="1:1">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" s="4"/>
     </row>
-    <row r="119" spans="1:1">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" s="4"/>
     </row>
-    <row r="120" spans="1:1">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" s="4"/>
     </row>
-    <row r="121" spans="1:1">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" s="4"/>
     </row>
-    <row r="122" spans="1:1">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" s="4"/>
     </row>
-    <row r="123" spans="1:1">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" s="4"/>
     </row>
-    <row r="124" spans="1:1">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" s="4"/>
     </row>
-    <row r="125" spans="1:1">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" s="4"/>
     </row>
-    <row r="126" spans="1:1">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" s="4"/>
     </row>
-    <row r="127" spans="1:1">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" s="4"/>
     </row>
-    <row r="128" spans="1:1">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" s="4"/>
     </row>
-    <row r="129" spans="1:4">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A129" s="12"/>
       <c r="B129" s="12"/>
       <c r="C129" s="11"/>
       <c r="D129" s="13"/>
     </row>
-    <row r="130" spans="1:4">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A130" s="15"/>
     </row>
-    <row r="131" spans="1:4">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" s="15"/>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" s="15"/>
     </row>
-    <row r="133" spans="1:4">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" s="15"/>
     </row>
-    <row r="134" spans="1:4">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" s="15"/>
     </row>
-    <row r="135" spans="1:4">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A135" s="15"/>
     </row>
-    <row r="136" spans="1:4">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A136" s="15"/>
     </row>
-    <row r="137" spans="1:4">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A137" s="15"/>
     </row>
-    <row r="138" spans="1:4">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A138" s="15"/>
     </row>
-    <row r="139" spans="1:4">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A139" s="15"/>
     </row>
-    <row r="140" spans="1:4">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A140" s="15"/>
     </row>
-    <row r="141" spans="1:4">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A141" s="15"/>
     </row>
-    <row r="142" spans="1:4">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A142" s="15"/>
     </row>
-    <row r="143" spans="1:4">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A143" s="15"/>
     </row>
-    <row r="144" spans="1:4">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A144" s="15"/>
     </row>
-    <row r="145" spans="1:4">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A145" s="15"/>
     </row>
-    <row r="146" spans="1:4">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A146" s="15"/>
     </row>
-    <row r="147" spans="1:4">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A147" s="12"/>
       <c r="B147" s="17"/>
       <c r="C147" s="17"/>
       <c r="D147" s="18"/>
     </row>
-    <row r="148" spans="1:4">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A148" s="20"/>
       <c r="B148" s="2"/>
       <c r="C148" s="2"/>
       <c r="D148" s="19"/>
     </row>
-    <row r="149" spans="1:4">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A149" s="20"/>
       <c r="B149" s="2"/>
       <c r="C149" s="2"/>
       <c r="D149" s="19"/>
     </row>
-    <row r="150" spans="1:4">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A150" s="20"/>
       <c r="B150" s="2"/>
       <c r="C150" s="2"/>
       <c r="D150" s="19"/>
     </row>
-    <row r="151" spans="1:4">
+    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A151" s="20"/>
       <c r="B151" s="2"/>
       <c r="C151" s="2"/>
       <c r="D151" s="19"/>
     </row>
-    <row r="152" spans="1:4">
+    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A152" s="20"/>
       <c r="B152" s="2"/>
       <c r="C152" s="2"/>
       <c r="D152" s="19"/>
     </row>
-    <row r="153" spans="1:4">
+    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A153" s="20"/>
       <c r="B153" s="2"/>
       <c r="C153" s="2"/>
       <c r="D153" s="19"/>
     </row>
-    <row r="154" spans="1:4">
+    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A154" s="20"/>
       <c r="B154" s="2"/>
       <c r="C154" s="2"/>
       <c r="D154" s="19"/>
     </row>
-    <row r="155" spans="1:4">
+    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A155" s="20"/>
       <c r="B155" s="2"/>
       <c r="C155" s="2"/>
       <c r="D155" s="19"/>
     </row>
-    <row r="156" spans="1:4">
+    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A156" s="20"/>
       <c r="B156" s="2"/>
       <c r="C156" s="2"/>
       <c r="D156" s="19"/>
     </row>
-    <row r="157" spans="1:4">
+    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A157" s="20"/>
       <c r="B157" s="2"/>
       <c r="C157" s="2"/>
       <c r="D157" s="19"/>
     </row>
-    <row r="158" spans="1:4">
+    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A158" s="20"/>
       <c r="B158" s="2"/>
       <c r="C158" s="2"/>
       <c r="D158" s="19"/>
     </row>
-    <row r="159" spans="1:4">
+    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A159" s="20"/>
       <c r="B159" s="2"/>
       <c r="C159" s="2"/>
       <c r="D159" s="19"/>
     </row>
-    <row r="160" spans="1:4">
+    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A160" s="20"/>
       <c r="B160" s="2"/>
       <c r="C160" s="2"/>
       <c r="D160" s="19"/>
     </row>
-    <row r="161" spans="1:4">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A161" s="20"/>
       <c r="B161" s="2"/>
       <c r="C161" s="2"/>
       <c r="D161" s="19"/>
     </row>
-    <row r="162" spans="1:4">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A162" s="20"/>
       <c r="B162" s="2"/>
       <c r="C162" s="2"/>
       <c r="D162" s="19"/>
     </row>
-    <row r="163" spans="1:4">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A163" s="20"/>
       <c r="B163" s="2"/>
       <c r="C163" s="2"/>
       <c r="D163" s="19"/>
     </row>
-    <row r="164" spans="1:4">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A164" s="20"/>
       <c r="B164" s="2"/>
       <c r="C164" s="2"/>
       <c r="D164" s="19"/>
     </row>
-    <row r="165" spans="1:4">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A165" s="12"/>
       <c r="B165" s="17"/>
       <c r="C165" s="17"/>
       <c r="D165" s="18"/>
     </row>
-    <row r="166" spans="1:4">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A166" s="15"/>
       <c r="B166" s="2"/>
       <c r="C166" s="2"/>
       <c r="D166" s="19"/>
     </row>
-    <row r="167" spans="1:4">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A167" s="15"/>
       <c r="B167" s="2"/>
       <c r="C167" s="2"/>
       <c r="D167" s="19"/>
     </row>
-    <row r="168" spans="1:4">
+    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A168" s="15"/>
       <c r="B168" s="2"/>
       <c r="C168" s="2"/>
       <c r="D168" s="19"/>
     </row>
-    <row r="169" spans="1:4">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A169" s="15"/>
       <c r="B169" s="2"/>
       <c r="C169" s="2"/>
       <c r="D169" s="19"/>
     </row>
-    <row r="170" spans="1:4">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A170" s="15"/>
       <c r="B170" s="2"/>
       <c r="C170" s="2"/>
       <c r="D170" s="19"/>
     </row>
-    <row r="171" spans="1:4">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A171" s="15"/>
       <c r="B171" s="2"/>
       <c r="C171" s="2"/>
       <c r="D171" s="19"/>
     </row>
-    <row r="172" spans="1:4">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A172" s="15"/>
       <c r="B172" s="2"/>
       <c r="C172" s="2"/>
       <c r="D172" s="19"/>
     </row>
-    <row r="173" spans="1:4">
+    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A173" s="15"/>
       <c r="B173" s="2"/>
       <c r="C173" s="2"/>
       <c r="D173" s="19"/>
     </row>
-    <row r="174" spans="1:4">
+    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A174" s="15"/>
       <c r="B174" s="2"/>
       <c r="C174" s="2"/>
       <c r="D174" s="19"/>
     </row>
-    <row r="175" spans="1:4">
+    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A175" s="15"/>
       <c r="B175" s="2"/>
       <c r="C175" s="2"/>
       <c r="D175" s="19"/>
     </row>
-    <row r="176" spans="1:4">
+    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A176" s="15"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
       <c r="D176" s="19"/>
     </row>
-    <row r="177" spans="1:4">
+    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A177" s="15"/>
       <c r="B177" s="2"/>
       <c r="C177" s="2"/>
       <c r="D177" s="19"/>
     </row>
-    <row r="178" spans="1:4">
+    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A178" s="15"/>
       <c r="B178" s="2"/>
       <c r="C178" s="2"/>
       <c r="D178" s="19"/>
     </row>
-    <row r="179" spans="1:4">
+    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A179" s="15"/>
       <c r="B179" s="2"/>
       <c r="C179" s="2"/>
       <c r="D179" s="19"/>
     </row>
-    <row r="180" spans="1:4">
+    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A180" s="15"/>
       <c r="B180" s="2"/>
       <c r="C180" s="2"/>
       <c r="D180" s="19"/>
     </row>
-    <row r="181" spans="1:4">
+    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A181" s="15"/>
       <c r="B181" s="2"/>
       <c r="C181" s="2"/>
       <c r="D181" s="19"/>
     </row>
-    <row r="182" spans="1:4">
+    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A182" s="15"/>
       <c r="B182" s="2"/>
       <c r="C182" s="2"/>
       <c r="D182" s="19"/>
     </row>
-    <row r="183" spans="1:4">
+    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A183" s="11"/>
       <c r="B183" s="17"/>
       <c r="C183" s="17"/>
       <c r="D183" s="18"/>
     </row>
-    <row r="184" spans="1:4">
+    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A184" s="16"/>
       <c r="B184" s="2"/>
       <c r="C184" s="2"/>
       <c r="D184" s="19"/>
     </row>
-    <row r="185" spans="1:4">
+    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A185" s="16"/>
       <c r="B185" s="2"/>
       <c r="C185" s="2"/>
       <c r="D185" s="19"/>
     </row>
-    <row r="186" spans="1:4">
+    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A186" s="16"/>
       <c r="B186" s="2"/>
       <c r="C186" s="2"/>
       <c r="D186" s="19"/>
     </row>
-    <row r="187" spans="1:4">
+    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A187" s="16"/>
       <c r="B187" s="2"/>
       <c r="C187" s="2"/>
       <c r="D187" s="19"/>
     </row>
-    <row r="188" spans="1:4">
+    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A188" s="16"/>
       <c r="B188" s="2"/>
       <c r="C188" s="2"/>
       <c r="D188" s="19"/>
     </row>
-    <row r="189" spans="1:4">
+    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A189" s="16"/>
       <c r="B189" s="2"/>
       <c r="C189" s="2"/>
       <c r="D189" s="19"/>
     </row>
-    <row r="190" spans="1:4">
+    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A190" s="16"/>
       <c r="B190" s="2"/>
       <c r="C190" s="2"/>
       <c r="D190" s="19"/>
     </row>
-    <row r="191" spans="1:4">
+    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A191" s="16"/>
       <c r="B191" s="2"/>
       <c r="C191" s="2"/>
       <c r="D191" s="19"/>
     </row>
-    <row r="192" spans="1:4">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A192" s="16"/>
       <c r="B192" s="2"/>
       <c r="C192" s="2"/>
       <c r="D192" s="19"/>
     </row>
-    <row r="193" spans="1:4">
+    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A193" s="16"/>
       <c r="B193" s="2"/>
       <c r="C193" s="2"/>
       <c r="D193" s="19"/>
     </row>
-    <row r="194" spans="1:4">
+    <row r="194" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A194" s="16"/>
       <c r="B194" s="2"/>
       <c r="C194" s="2"/>
       <c r="D194" s="19"/>
     </row>
-    <row r="195" spans="1:4">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A195" s="16"/>
       <c r="B195" s="2"/>
       <c r="C195" s="2"/>
       <c r="D195" s="19"/>
     </row>
-    <row r="196" spans="1:4">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A196" s="16"/>
       <c r="B196" s="2"/>
       <c r="C196" s="2"/>
       <c r="D196" s="19"/>
     </row>
-    <row r="197" spans="1:4">
+    <row r="197" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A197" s="16"/>
       <c r="B197" s="2"/>
       <c r="C197" s="2"/>
       <c r="D197" s="19"/>
     </row>
-    <row r="198" spans="1:4">
+    <row r="198" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A198" s="16"/>
       <c r="B198" s="2"/>
       <c r="C198" s="2"/>
       <c r="D198" s="19"/>
     </row>
-    <row r="199" spans="1:4">
+    <row r="199" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A199" s="16"/>
       <c r="B199" s="2"/>
       <c r="C199" s="2"/>
       <c r="D199" s="19"/>
     </row>
-    <row r="200" spans="1:4">
+    <row r="200" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A200" s="16"/>
       <c r="B200" s="2"/>
       <c r="C200" s="2"/>
       <c r="D200" s="19"/>
     </row>
-    <row r="201" spans="1:4">
+    <row r="201" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A201" s="11"/>
       <c r="B201" s="17"/>
       <c r="C201" s="17"/>
       <c r="D201" s="18"/>
     </row>
-    <row r="202" spans="1:4">
+    <row r="202" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A202" s="16"/>
       <c r="B202" s="2"/>
       <c r="C202" s="2"/>
       <c r="D202" s="19"/>
     </row>
-    <row r="203" spans="1:4">
+    <row r="203" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A203" s="16"/>
       <c r="B203" s="2"/>
       <c r="C203" s="2"/>
       <c r="D203" s="19"/>
     </row>
-    <row r="204" spans="1:4">
+    <row r="204" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A204" s="16"/>
       <c r="B204" s="2"/>
       <c r="C204" s="2"/>
       <c r="D204" s="19"/>
     </row>
-    <row r="205" spans="1:4">
+    <row r="205" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A205" s="16"/>
       <c r="B205" s="2"/>
       <c r="C205" s="2"/>
       <c r="D205" s="19"/>
     </row>
-    <row r="206" spans="1:4">
+    <row r="206" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A206" s="16"/>
       <c r="B206" s="2"/>
       <c r="C206" s="2"/>
       <c r="D206" s="19"/>
     </row>
-    <row r="207" spans="1:4">
+    <row r="207" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A207" s="16"/>
       <c r="B207" s="2"/>
       <c r="C207" s="2"/>
       <c r="D207" s="19"/>
     </row>
-    <row r="208" spans="1:4">
+    <row r="208" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A208" s="16"/>
       <c r="B208" s="2"/>
       <c r="C208" s="2"/>
       <c r="D208" s="19"/>
     </row>
-    <row r="209" spans="1:4">
+    <row r="209" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A209" s="16"/>
       <c r="B209" s="2"/>
       <c r="C209" s="2"/>
       <c r="D209" s="19"/>
     </row>
-    <row r="210" spans="1:4">
+    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A210" s="16"/>
       <c r="B210" s="2"/>
       <c r="C210" s="2"/>
       <c r="D210" s="19"/>
     </row>
-    <row r="211" spans="1:4">
+    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A211" s="16"/>
       <c r="B211" s="2"/>
       <c r="C211" s="2"/>
       <c r="D211" s="19"/>
     </row>
-    <row r="212" spans="1:4">
+    <row r="212" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A212" s="16"/>
       <c r="B212" s="2"/>
       <c r="C212" s="2"/>
       <c r="D212" s="19"/>
     </row>
-    <row r="213" spans="1:4">
+    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A213" s="16"/>
       <c r="B213" s="2"/>
       <c r="C213" s="2"/>
       <c r="D213" s="19"/>
     </row>
-    <row r="214" spans="1:4">
+    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A214" s="16"/>
       <c r="B214" s="2"/>
       <c r="C214" s="2"/>
       <c r="D214" s="19"/>
     </row>
-    <row r="215" spans="1:4">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A215" s="16"/>
       <c r="B215" s="2"/>
       <c r="C215" s="2"/>
       <c r="D215" s="19"/>
     </row>
-    <row r="216" spans="1:4">
+    <row r="216" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A216" s="16"/>
       <c r="B216" s="2"/>
       <c r="C216" s="2"/>
       <c r="D216" s="19"/>
     </row>
-    <row r="217" spans="1:4">
+    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A217" s="16"/>
       <c r="B217" s="2"/>
       <c r="C217" s="2"/>
       <c r="D217" s="19"/>
     </row>
-    <row r="218" spans="1:4">
+    <row r="218" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A218" s="16"/>
       <c r="B218" s="2"/>
       <c r="C218" s="2"/>
       <c r="D218" s="19"/>
     </row>
-    <row r="219" spans="1:4">
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A219" s="11"/>
       <c r="B219" s="17"/>
       <c r="C219" s="17"/>
       <c r="D219" s="18"/>
     </row>
-    <row r="220" spans="1:4">
+    <row r="220" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A220" s="14"/>
       <c r="B220" s="2"/>
       <c r="C220" s="2"/>
       <c r="D220" s="19"/>
     </row>
-    <row r="221" spans="1:4">
+    <row r="221" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A221" s="14"/>
       <c r="B221" s="2"/>
       <c r="C221" s="2"/>
       <c r="D221" s="19"/>
     </row>
-    <row r="222" spans="1:4">
+    <row r="222" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A222" s="14"/>
       <c r="B222" s="2"/>
       <c r="C222" s="2"/>
       <c r="D222" s="19"/>
     </row>
-    <row r="223" spans="1:4">
+    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A223" s="14"/>
       <c r="B223" s="2"/>
       <c r="C223" s="2"/>
       <c r="D223" s="19"/>
     </row>
-    <row r="224" spans="1:4">
+    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A224" s="14"/>
       <c r="B224" s="2"/>
       <c r="C224" s="2"/>
       <c r="D224" s="19"/>
     </row>
-    <row r="225" spans="1:4">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A225" s="14"/>
       <c r="B225" s="2"/>
       <c r="C225" s="2"/>
       <c r="D225" s="19"/>
     </row>
-    <row r="226" spans="1:4">
+    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A226" s="14"/>
       <c r="B226" s="2"/>
       <c r="C226" s="2"/>
       <c r="D226" s="19"/>
     </row>
-    <row r="227" spans="1:4">
+    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A227" s="14"/>
       <c r="B227" s="2"/>
       <c r="C227" s="2"/>
       <c r="D227" s="19"/>
     </row>
-    <row r="228" spans="1:4">
+    <row r="228" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A228" s="14"/>
       <c r="B228" s="2"/>
       <c r="C228" s="2"/>
       <c r="D228" s="19"/>
     </row>
-    <row r="229" spans="1:4">
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A229" s="14"/>
       <c r="B229" s="2"/>
       <c r="C229" s="2"/>
       <c r="D229" s="19"/>
     </row>
-    <row r="230" spans="1:4">
+    <row r="230" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A230" s="14"/>
       <c r="B230" s="2"/>
       <c r="C230" s="2"/>
       <c r="D230" s="19"/>
     </row>
-    <row r="231" spans="1:4">
+    <row r="231" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A231" s="14"/>
       <c r="B231" s="2"/>
       <c r="C231" s="2"/>
       <c r="D231" s="19"/>
     </row>
-    <row r="232" spans="1:4">
+    <row r="232" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A232" s="14"/>
       <c r="B232" s="2"/>
       <c r="C232" s="2"/>
       <c r="D232" s="19"/>
     </row>
-    <row r="233" spans="1:4">
+    <row r="233" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A233" s="14"/>
       <c r="B233" s="2"/>
       <c r="C233" s="2"/>
       <c r="D233" s="19"/>
     </row>
-    <row r="234" spans="1:4">
+    <row r="234" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A234" s="14"/>
       <c r="B234" s="2"/>
       <c r="C234" s="2"/>
       <c r="D234" s="19"/>
     </row>
-    <row r="235" spans="1:4">
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A235" s="14"/>
       <c r="B235" s="2"/>
       <c r="C235" s="2"/>
       <c r="D235" s="19"/>
     </row>
-    <row r="236" spans="1:4">
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A236" s="14"/>
       <c r="B236" s="2"/>
       <c r="C236" s="2"/>
       <c r="D236" s="19"/>
     </row>
-    <row r="237" spans="1:4">
+    <row r="237" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A237" s="11"/>
       <c r="B237" s="17"/>
       <c r="C237" s="17"/>
       <c r="D237" s="18"/>
     </row>
-    <row r="238" spans="1:4">
+    <row r="238" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A238" s="14"/>
       <c r="B238" s="2"/>
       <c r="C238" s="2"/>
       <c r="D238" s="19"/>
     </row>
-    <row r="239" spans="1:4">
+    <row r="239" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A239" s="14"/>
       <c r="B239" s="2"/>
       <c r="C239" s="2"/>
       <c r="D239" s="19"/>
     </row>
-    <row r="240" spans="1:4">
+    <row r="240" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A240" s="14"/>
       <c r="B240" s="2"/>
       <c r="C240" s="2"/>
       <c r="D240" s="19"/>
     </row>
-    <row r="241" spans="1:4">
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A241" s="14"/>
       <c r="B241" s="2"/>
       <c r="C241" s="2"/>
       <c r="D241" s="19"/>
     </row>
-    <row r="242" spans="1:4">
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A242" s="14"/>
       <c r="B242" s="2"/>
       <c r="C242" s="2"/>
       <c r="D242" s="19"/>
     </row>
-    <row r="243" spans="1:4">
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A243" s="14"/>
       <c r="B243" s="2"/>
       <c r="C243" s="2"/>
       <c r="D243" s="19"/>
     </row>
-    <row r="244" spans="1:4">
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A244" s="14"/>
       <c r="B244" s="2"/>
       <c r="C244" s="2"/>
       <c r="D244" s="19"/>
     </row>
-    <row r="245" spans="1:4">
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A245" s="14"/>
       <c r="B245" s="2"/>
       <c r="C245" s="2"/>
       <c r="D245" s="19"/>
     </row>
-    <row r="246" spans="1:4">
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A246" s="14"/>
       <c r="B246" s="2"/>
       <c r="C246" s="2"/>
       <c r="D246" s="19"/>
     </row>
-    <row r="247" spans="1:4">
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A247" s="14"/>
       <c r="B247" s="2"/>
       <c r="C247" s="2"/>
       <c r="D247" s="19"/>
     </row>
-    <row r="248" spans="1:4">
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A248" s="14"/>
       <c r="B248" s="2"/>
       <c r="C248" s="2"/>
       <c r="D248" s="19"/>
     </row>
-    <row r="249" spans="1:4">
+    <row r="249" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A249" s="14"/>
       <c r="B249" s="2"/>
       <c r="C249" s="2"/>
       <c r="D249" s="19"/>
     </row>
-    <row r="250" spans="1:4">
+    <row r="250" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A250" s="14"/>
       <c r="B250" s="2"/>
       <c r="C250" s="2"/>
       <c r="D250" s="19"/>
     </row>
-    <row r="251" spans="1:4">
+    <row r="251" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A251" s="14"/>
       <c r="B251" s="2"/>
       <c r="C251" s="2"/>
       <c r="D251" s="19"/>
     </row>
-    <row r="252" spans="1:4">
+    <row r="252" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A252" s="14"/>
       <c r="B252" s="2"/>
       <c r="C252" s="2"/>
       <c r="D252" s="19"/>
     </row>
-    <row r="253" spans="1:4">
+    <row r="253" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A253" s="14"/>
       <c r="B253" s="2"/>
       <c r="C253" s="2"/>
       <c r="D253" s="19"/>
     </row>
-    <row r="254" spans="1:4">
+    <row r="254" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A254" s="14"/>
       <c r="B254" s="2"/>
       <c r="C254" s="2"/>
       <c r="D254" s="19"/>
     </row>
-    <row r="255" spans="1:4">
+    <row r="255" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A255" s="11"/>
       <c r="B255" s="17"/>
       <c r="C255" s="17"/>
       <c r="D255" s="18"/>
     </row>
-    <row r="256" spans="1:4">
+    <row r="256" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B256" s="2"/>
       <c r="C256" s="2"/>
       <c r="D256" s="19"/>
     </row>
-    <row r="257" spans="2:4">
+    <row r="257" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B257" s="2"/>
       <c r="C257" s="2"/>
       <c r="D257" s="19"/>
     </row>
-    <row r="258" spans="2:4">
+    <row r="258" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B258" s="2"/>
       <c r="C258" s="2"/>
       <c r="D258" s="19"/>
     </row>
-    <row r="259" spans="2:4">
+    <row r="259" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B259" s="2"/>
       <c r="C259" s="2"/>
       <c r="D259" s="19"/>
     </row>
-    <row r="260" spans="2:4">
+    <row r="260" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B260" s="2"/>
       <c r="C260" s="2"/>
       <c r="D260" s="19"/>
     </row>
-    <row r="261" spans="2:4">
+    <row r="261" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B261" s="2"/>
       <c r="C261" s="2"/>
       <c r="D261" s="19"/>
     </row>
-    <row r="262" spans="2:4">
+    <row r="262" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B262" s="2"/>
       <c r="C262" s="2"/>
       <c r="D262" s="19"/>
     </row>
-    <row r="263" spans="2:4">
+    <row r="263" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B263" s="2"/>
       <c r="C263" s="2"/>
       <c r="D263" s="19"/>
     </row>
-    <row r="264" spans="2:4">
+    <row r="264" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B264" s="2"/>
       <c r="C264" s="2"/>
       <c r="D264" s="19"/>
     </row>
-    <row r="265" spans="2:4">
+    <row r="265" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B265" s="2"/>
       <c r="C265" s="2"/>
       <c r="D265" s="19"/>
     </row>
-    <row r="266" spans="2:4">
+    <row r="266" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B266" s="2"/>
       <c r="C266" s="2"/>
       <c r="D266" s="19"/>
     </row>
-    <row r="267" spans="2:4">
+    <row r="267" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B267" s="2"/>
       <c r="C267" s="2"/>
       <c r="D267" s="19"/>
     </row>
-    <row r="268" spans="2:4">
+    <row r="268" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B268" s="2"/>
       <c r="C268" s="2"/>
       <c r="D268" s="19"/>
     </row>
-    <row r="269" spans="2:4">
+    <row r="269" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B269" s="2"/>
       <c r="C269" s="2"/>
       <c r="D269" s="19"/>
     </row>
-    <row r="270" spans="2:4">
+    <row r="270" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B270" s="2"/>
       <c r="C270" s="2"/>
       <c r="D270" s="19"/>
     </row>
-    <row r="271" spans="2:4">
+    <row r="271" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B271" s="2"/>
       <c r="C271" s="2"/>
       <c r="D271" s="19"/>
     </row>
-    <row r="272" spans="2:4">
+    <row r="272" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B272" s="2"/>
       <c r="C272" s="2"/>
       <c r="D272" s="19"/>
     </row>
-    <row r="273" spans="1:4">
+    <row r="273" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A273" s="11"/>
       <c r="B273" s="17"/>
       <c r="C273" s="17"/>
       <c r="D273" s="18"/>
     </row>
-    <row r="274" spans="1:4">
+    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B274" s="2"/>
       <c r="C274" s="2"/>
       <c r="D274" s="19"/>
     </row>
-    <row r="275" spans="1:4">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B275" s="2"/>
       <c r="C275" s="2"/>
       <c r="D275" s="19"/>
     </row>
-    <row r="276" spans="1:4">
+    <row r="276" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B276" s="2"/>
       <c r="C276" s="2"/>
       <c r="D276" s="19"/>
     </row>
-    <row r="277" spans="1:4">
+    <row r="277" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B277" s="2"/>
       <c r="C277" s="2"/>
       <c r="D277" s="19"/>
     </row>
-    <row r="278" spans="1:4">
+    <row r="278" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B278" s="2"/>
       <c r="C278" s="2"/>
       <c r="D278" s="19"/>
     </row>
-    <row r="279" spans="1:4">
+    <row r="279" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B279" s="2"/>
       <c r="C279" s="2"/>
       <c r="D279" s="19"/>
     </row>
-    <row r="280" spans="1:4">
+    <row r="280" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B280" s="2"/>
       <c r="C280" s="2"/>
       <c r="D280" s="19"/>
     </row>
-    <row r="281" spans="1:4">
+    <row r="281" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B281" s="2"/>
       <c r="C281" s="2"/>
       <c r="D281" s="19"/>
     </row>
-    <row r="282" spans="1:4">
+    <row r="282" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B282" s="2"/>
       <c r="C282" s="2"/>
       <c r="D282" s="19"/>
     </row>
-    <row r="283" spans="1:4">
+    <row r="283" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B283" s="2"/>
       <c r="C283" s="2"/>
       <c r="D283" s="19"/>
     </row>
-    <row r="284" spans="1:4">
+    <row r="284" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B284" s="2"/>
       <c r="C284" s="2"/>
       <c r="D284" s="19"/>
     </row>
-    <row r="285" spans="1:4">
+    <row r="285" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B285" s="2"/>
       <c r="C285" s="2"/>
       <c r="D285" s="19"/>
     </row>
-    <row r="286" spans="1:4">
+    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B286" s="2"/>
       <c r="C286" s="2"/>
       <c r="D286" s="19"/>
     </row>
-    <row r="287" spans="1:4">
+    <row r="287" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B287" s="2"/>
       <c r="C287" s="2"/>
       <c r="D287" s="19"/>
     </row>
-    <row r="288" spans="1:4">
+    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B288" s="2"/>
       <c r="C288" s="2"/>
       <c r="D288" s="19"/>
     </row>
-    <row r="289" spans="1:4">
+    <row r="289" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B289" s="2"/>
       <c r="C289" s="2"/>
       <c r="D289" s="19"/>
     </row>
-    <row r="290" spans="1:4">
+    <row r="290" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B290" s="2"/>
       <c r="C290" s="2"/>
       <c r="D290" s="19"/>
     </row>
-    <row r="291" spans="1:4">
+    <row r="291" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A291" s="11"/>
       <c r="B291" s="17"/>
       <c r="C291" s="17"/>
       <c r="D291" s="18"/>
     </row>
-    <row r="292" spans="1:4">
+    <row r="292" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B292" s="2"/>
       <c r="C292" s="2"/>
       <c r="D292" s="19"/>
     </row>
-    <row r="293" spans="1:4">
+    <row r="293" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B293" s="2"/>
       <c r="C293" s="2"/>
       <c r="D293" s="19"/>
     </row>
-    <row r="294" spans="1:4">
+    <row r="294" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B294" s="2"/>
       <c r="C294" s="2"/>
       <c r="D294" s="19"/>
     </row>
-    <row r="295" spans="1:4">
+    <row r="295" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B295" s="2"/>
       <c r="C295" s="2"/>
       <c r="D295" s="19"/>
     </row>
-    <row r="296" spans="1:4">
+    <row r="296" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B296" s="2"/>
       <c r="C296" s="2"/>
       <c r="D296" s="19"/>
     </row>
-    <row r="297" spans="1:4">
+    <row r="297" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B297" s="2"/>
       <c r="C297" s="2"/>
       <c r="D297" s="19"/>
     </row>
-    <row r="298" spans="1:4">
+    <row r="298" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B298" s="2"/>
       <c r="C298" s="2"/>
       <c r="D298" s="19"/>
     </row>
-    <row r="299" spans="1:4">
+    <row r="299" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B299" s="2"/>
       <c r="C299" s="2"/>
       <c r="D299" s="19"/>
     </row>
-    <row r="300" spans="1:4">
+    <row r="300" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B300" s="2"/>
       <c r="C300" s="2"/>
       <c r="D300" s="19"/>
     </row>
-    <row r="301" spans="1:4">
+    <row r="301" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B301" s="2"/>
       <c r="C301" s="2"/>
       <c r="D301" s="19"/>
     </row>
-    <row r="302" spans="1:4">
+    <row r="302" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B302" s="2"/>
       <c r="C302" s="2"/>
       <c r="D302" s="19"/>
     </row>
-    <row r="303" spans="1:4">
+    <row r="303" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B303" s="2"/>
       <c r="C303" s="2"/>
       <c r="D303" s="19"/>
     </row>
-    <row r="304" spans="1:4">
+    <row r="304" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B304" s="2"/>
       <c r="C304" s="2"/>
       <c r="D304" s="19"/>
     </row>
-    <row r="305" spans="1:4">
+    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B305" s="2"/>
       <c r="C305" s="2"/>
       <c r="D305" s="19"/>
     </row>
-    <row r="306" spans="1:4">
+    <row r="306" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B306" s="2"/>
       <c r="C306" s="2"/>
       <c r="D306" s="19"/>
     </row>
-    <row r="307" spans="1:4">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B307" s="2"/>
       <c r="C307" s="2"/>
       <c r="D307" s="19"/>
     </row>
-    <row r="308" spans="1:4">
+    <row r="308" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B308" s="2"/>
       <c r="C308" s="2"/>
       <c r="D308" s="19"/>
     </row>
-    <row r="309" spans="1:4">
+    <row r="309" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A309" s="11"/>
       <c r="B309" s="17"/>
       <c r="C309" s="17"/>
       <c r="D309" s="18"/>
     </row>
-    <row r="310" spans="1:4">
+    <row r="310" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B310" s="2"/>
       <c r="C310" s="2"/>
       <c r="D310" s="19"/>
     </row>
-    <row r="311" spans="1:4">
+    <row r="311" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B311" s="2"/>
       <c r="C311" s="2"/>
       <c r="D311" s="19"/>
     </row>
-    <row r="312" spans="1:4">
+    <row r="312" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B312" s="2"/>
       <c r="C312" s="2"/>
       <c r="D312" s="19"/>
     </row>
-    <row r="313" spans="1:4">
+    <row r="313" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B313" s="2"/>
       <c r="C313" s="2"/>
       <c r="D313" s="19"/>
     </row>
-    <row r="314" spans="1:4">
+    <row r="314" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B314" s="2"/>
       <c r="C314" s="2"/>
       <c r="D314" s="19"/>
     </row>
-    <row r="315" spans="1:4">
+    <row r="315" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B315" s="2"/>
       <c r="C315" s="2"/>
       <c r="D315" s="19"/>
     </row>
-    <row r="316" spans="1:4">
+    <row r="316" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B316" s="2"/>
       <c r="C316" s="2"/>
       <c r="D316" s="19"/>
     </row>
-    <row r="317" spans="1:4">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B317" s="2"/>
       <c r="C317" s="2"/>
       <c r="D317" s="19"/>
     </row>
-    <row r="318" spans="1:4">
+    <row r="318" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B318" s="2"/>
       <c r="C318" s="2"/>
       <c r="D318" s="19"/>
     </row>
-    <row r="319" spans="1:4">
+    <row r="319" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B319" s="2"/>
       <c r="C319" s="2"/>
       <c r="D319" s="19"/>
     </row>
-    <row r="320" spans="1:4">
+    <row r="320" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B320" s="2"/>
       <c r="C320" s="2"/>
       <c r="D320" s="19"/>
     </row>
-    <row r="321" spans="1:4">
+    <row r="321" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B321" s="2"/>
       <c r="C321" s="2"/>
       <c r="D321" s="19"/>
     </row>
-    <row r="322" spans="1:4">
+    <row r="322" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B322" s="2"/>
       <c r="C322" s="2"/>
       <c r="D322" s="19"/>
     </row>
-    <row r="323" spans="1:4">
+    <row r="323" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B323" s="2"/>
       <c r="C323" s="2"/>
       <c r="D323" s="19"/>
     </row>
-    <row r="324" spans="1:4">
+    <row r="324" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B324" s="2"/>
       <c r="C324" s="2"/>
       <c r="D324" s="19"/>
     </row>
-    <row r="325" spans="1:4">
+    <row r="325" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B325" s="2"/>
       <c r="C325" s="2"/>
       <c r="D325" s="19"/>
     </row>
-    <row r="326" spans="1:4">
+    <row r="326" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B326" s="2"/>
       <c r="C326" s="2"/>
       <c r="D326" s="19"/>
     </row>
-    <row r="327" spans="1:4">
+    <row r="327" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A327" s="11"/>
       <c r="B327" s="17"/>
       <c r="C327" s="17"/>
       <c r="D327" s="18"/>
     </row>
-    <row r="328" spans="1:4">
+    <row r="328" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B328" s="2"/>
       <c r="C328" s="2"/>
       <c r="D328" s="19"/>
     </row>
-    <row r="329" spans="1:4">
+    <row r="329" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B329" s="2"/>
       <c r="C329" s="2"/>
       <c r="D329" s="19"/>
     </row>
-    <row r="330" spans="1:4">
+    <row r="330" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B330" s="2"/>
       <c r="C330" s="2"/>
       <c r="D330" s="19"/>
     </row>
-    <row r="331" spans="1:4">
+    <row r="331" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B331" s="2"/>
       <c r="C331" s="2"/>
       <c r="D331" s="19"/>
     </row>
-    <row r="332" spans="1:4">
+    <row r="332" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B332" s="2"/>
       <c r="C332" s="2"/>
       <c r="D332" s="19"/>
     </row>
-    <row r="333" spans="1:4">
+    <row r="333" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B333" s="2"/>
       <c r="C333" s="2"/>
       <c r="D333" s="19"/>
     </row>
-    <row r="334" spans="1:4">
+    <row r="334" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B334" s="2"/>
       <c r="C334" s="2"/>
       <c r="D334" s="19"/>
     </row>
-    <row r="335" spans="1:4">
+    <row r="335" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B335" s="2"/>
       <c r="C335" s="2"/>
       <c r="D335" s="19"/>
     </row>
-    <row r="336" spans="1:4">
+    <row r="336" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B336" s="2"/>
       <c r="C336" s="2"/>
       <c r="D336" s="19"/>
     </row>
-    <row r="337" spans="1:4">
+    <row r="337" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B337" s="2"/>
       <c r="C337" s="2"/>
       <c r="D337" s="19"/>
     </row>
-    <row r="338" spans="1:4">
+    <row r="338" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B338" s="2"/>
       <c r="C338" s="2"/>
       <c r="D338" s="19"/>
     </row>
-    <row r="339" spans="1:4">
+    <row r="339" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B339" s="2"/>
       <c r="C339" s="2"/>
       <c r="D339" s="19"/>
     </row>
-    <row r="340" spans="1:4">
+    <row r="340" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B340" s="2"/>
       <c r="C340" s="2"/>
       <c r="D340" s="19"/>
     </row>
-    <row r="341" spans="1:4">
+    <row r="341" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B341" s="2"/>
       <c r="C341" s="2"/>
       <c r="D341" s="19"/>
     </row>
-    <row r="342" spans="1:4">
+    <row r="342" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B342" s="2"/>
       <c r="C342" s="2"/>
       <c r="D342" s="19"/>
     </row>
-    <row r="343" spans="1:4">
+    <row r="343" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B343" s="2"/>
       <c r="C343" s="2"/>
       <c r="D343" s="19"/>
     </row>
-    <row r="344" spans="1:4">
+    <row r="344" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B344" s="2"/>
       <c r="C344" s="2"/>
       <c r="D344" s="19"/>
     </row>
-    <row r="345" spans="1:4">
+    <row r="345" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A345" s="11"/>
       <c r="B345" s="17"/>
       <c r="C345" s="17"/>
       <c r="D345" s="18"/>
     </row>
-    <row r="346" spans="1:4">
+    <row r="346" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B346" s="2"/>
       <c r="C346" s="2"/>
     </row>
-    <row r="347" spans="1:4">
+    <row r="347" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B347" s="2"/>
       <c r="C347" s="2"/>
     </row>
-    <row r="348" spans="1:4">
+    <row r="348" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B348" s="2"/>
       <c r="C348" s="2"/>
     </row>
-    <row r="349" spans="1:4">
+    <row r="349" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B349" s="2"/>
       <c r="C349" s="2"/>
     </row>
-    <row r="350" spans="1:4">
+    <row r="350" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B350" s="2"/>
       <c r="C350" s="2"/>
     </row>
-    <row r="351" spans="1:4">
+    <row r="351" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B351" s="2"/>
       <c r="C351" s="2"/>
     </row>
-    <row r="352" spans="1:4">
+    <row r="352" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B352" s="2"/>
       <c r="C352" s="2"/>
     </row>
-    <row r="353" spans="1:4">
+    <row r="353" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B353" s="2"/>
       <c r="C353" s="2"/>
     </row>
-    <row r="354" spans="1:4">
+    <row r="354" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B354" s="2"/>
       <c r="C354" s="2"/>
     </row>
-    <row r="355" spans="1:4">
+    <row r="355" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B355" s="2"/>
       <c r="C355" s="2"/>
     </row>
-    <row r="356" spans="1:4">
+    <row r="356" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B356" s="2"/>
       <c r="C356" s="2"/>
     </row>
-    <row r="357" spans="1:4">
+    <row r="357" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B357" s="2"/>
       <c r="C357" s="2"/>
     </row>
-    <row r="358" spans="1:4">
+    <row r="358" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B358" s="2"/>
       <c r="C358" s="2"/>
     </row>
-    <row r="359" spans="1:4">
+    <row r="359" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B359" s="2"/>
       <c r="C359" s="2"/>
     </row>
-    <row r="360" spans="1:4">
+    <row r="360" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B360" s="2"/>
       <c r="C360" s="2"/>
     </row>
-    <row r="361" spans="1:4">
+    <row r="361" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B361" s="2"/>
       <c r="C361" s="2"/>
     </row>
-    <row r="362" spans="1:4">
+    <row r="362" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B362" s="2"/>
       <c r="C362" s="2"/>
     </row>
-    <row r="363" spans="1:4">
+    <row r="363" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A363" s="11"/>
       <c r="B363" s="17"/>
       <c r="C363" s="17"/>
       <c r="D363" s="18"/>
     </row>
-    <row r="364" spans="1:4">
+    <row r="364" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B364" s="2"/>
       <c r="C364" s="2"/>
     </row>
-    <row r="365" spans="1:4">
+    <row r="365" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B365" s="2"/>
       <c r="C365" s="2"/>
     </row>
-    <row r="366" spans="1:4">
+    <row r="366" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B366" s="2"/>
       <c r="C366" s="2"/>
     </row>
-    <row r="367" spans="1:4">
+    <row r="367" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B367" s="2"/>
       <c r="C367" s="2"/>
     </row>
-    <row r="368" spans="1:4">
+    <row r="368" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B368" s="2"/>
       <c r="C368" s="2"/>
     </row>
-    <row r="369" spans="1:4">
+    <row r="369" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B369" s="2"/>
       <c r="C369" s="2"/>
     </row>
-    <row r="370" spans="1:4">
+    <row r="370" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B370" s="2"/>
       <c r="C370" s="2"/>
     </row>
-    <row r="371" spans="1:4">
+    <row r="371" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B371" s="2"/>
       <c r="C371" s="2"/>
     </row>
-    <row r="372" spans="1:4">
+    <row r="372" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B372" s="2"/>
       <c r="C372" s="2"/>
     </row>
-    <row r="373" spans="1:4">
+    <row r="373" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B373" s="2"/>
       <c r="C373" s="2"/>
     </row>
-    <row r="374" spans="1:4">
+    <row r="374" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B374" s="2"/>
       <c r="C374" s="2"/>
     </row>
-    <row r="375" spans="1:4">
+    <row r="375" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B375" s="2"/>
       <c r="C375" s="2"/>
     </row>
-    <row r="376" spans="1:4">
+    <row r="376" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B376" s="2"/>
       <c r="C376" s="2"/>
     </row>
-    <row r="377" spans="1:4">
+    <row r="377" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B377" s="2"/>
       <c r="C377" s="2"/>
     </row>
-    <row r="378" spans="1:4">
+    <row r="378" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B378" s="2"/>
       <c r="C378" s="2"/>
     </row>
-    <row r="379" spans="1:4">
+    <row r="379" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B379" s="2"/>
       <c r="C379" s="2"/>
     </row>
-    <row r="380" spans="1:4">
+    <row r="380" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B380" s="2"/>
       <c r="C380" s="2"/>
     </row>
-    <row r="381" spans="1:4">
+    <row r="381" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A381" s="11"/>
       <c r="B381" s="17"/>
       <c r="C381" s="17"/>
       <c r="D381" s="18"/>
     </row>
-    <row r="382" spans="1:4">
+    <row r="382" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B382" s="2"/>
       <c r="C382" s="2"/>
     </row>
-    <row r="383" spans="1:4">
+    <row r="383" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B383" s="2"/>
       <c r="C383" s="2"/>
     </row>
-    <row r="384" spans="1:4">
+    <row r="384" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B384" s="2"/>
       <c r="C384" s="2"/>
     </row>
-    <row r="385" spans="1:4">
+    <row r="385" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B385" s="2"/>
       <c r="C385" s="2"/>
     </row>
-    <row r="386" spans="1:4">
+    <row r="386" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B386" s="2"/>
       <c r="C386" s="2"/>
     </row>
-    <row r="387" spans="1:4">
+    <row r="387" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B387" s="2"/>
       <c r="C387" s="2"/>
     </row>
-    <row r="388" spans="1:4">
+    <row r="388" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B388" s="2"/>
       <c r="C388" s="2"/>
     </row>
-    <row r="389" spans="1:4">
+    <row r="389" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B389" s="2"/>
       <c r="C389" s="2"/>
     </row>
-    <row r="390" spans="1:4">
+    <row r="390" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B390" s="2"/>
       <c r="C390" s="2"/>
     </row>
-    <row r="391" spans="1:4">
+    <row r="391" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B391" s="2"/>
       <c r="C391" s="2"/>
     </row>
-    <row r="392" spans="1:4">
+    <row r="392" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B392" s="2"/>
       <c r="C392" s="2"/>
     </row>
-    <row r="393" spans="1:4">
+    <row r="393" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B393" s="2"/>
       <c r="C393" s="2"/>
     </row>
-    <row r="394" spans="1:4">
+    <row r="394" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B394" s="2"/>
       <c r="C394" s="2"/>
     </row>
-    <row r="395" spans="1:4">
+    <row r="395" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B395" s="2"/>
       <c r="C395" s="2"/>
     </row>
-    <row r="396" spans="1:4">
+    <row r="396" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B396" s="2"/>
       <c r="C396" s="2"/>
     </row>
-    <row r="397" spans="1:4">
+    <row r="397" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B397" s="2"/>
       <c r="C397" s="2"/>
     </row>
-    <row r="398" spans="1:4">
+    <row r="398" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B398" s="2"/>
       <c r="C398" s="2"/>
     </row>
-    <row r="399" spans="1:4">
+    <row r="399" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A399" s="11"/>
       <c r="B399" s="17"/>
       <c r="C399" s="17"/>
       <c r="D399" s="18"/>
     </row>
-    <row r="400" spans="1:4">
+    <row r="400" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B400" s="2"/>
       <c r="C400" s="2"/>
     </row>
-    <row r="401" spans="2:3">
+    <row r="401" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B401" s="2"/>
       <c r="C401" s="2"/>
     </row>
-    <row r="402" spans="2:3">
+    <row r="402" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B402" s="2"/>
       <c r="C402" s="2"/>
     </row>
-    <row r="403" spans="2:3">
+    <row r="403" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B403" s="2"/>
       <c r="C403" s="2"/>
     </row>
-    <row r="404" spans="2:3">
+    <row r="404" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B404" s="2"/>
       <c r="C404" s="2"/>
     </row>
-    <row r="405" spans="2:3">
+    <row r="405" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B405" s="2"/>
       <c r="C405" s="2"/>
     </row>
-    <row r="406" spans="2:3">
+    <row r="406" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B406" s="2"/>
       <c r="C406" s="2"/>
     </row>
-    <row r="407" spans="2:3">
+    <row r="407" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B407" s="2"/>
       <c r="C407" s="2"/>
     </row>
-    <row r="408" spans="2:3">
+    <row r="408" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B408" s="2"/>
       <c r="C408" s="2"/>
     </row>
-    <row r="409" spans="2:3">
+    <row r="409" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B409" s="2"/>
       <c r="C409" s="2"/>
     </row>
-    <row r="410" spans="2:3">
+    <row r="410" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B410" s="2"/>
       <c r="C410" s="2"/>
     </row>
-    <row r="411" spans="2:3">
+    <row r="411" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B411" s="2"/>
       <c r="C411" s="2"/>
     </row>
-    <row r="412" spans="2:3">
+    <row r="412" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B412" s="2"/>
       <c r="C412" s="2"/>
     </row>
-    <row r="413" spans="2:3">
+    <row r="413" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B413" s="2"/>
       <c r="C413" s="2"/>
     </row>
-    <row r="414" spans="2:3">
+    <row r="414" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B414" s="2"/>
       <c r="C414" s="2"/>
     </row>
-    <row r="415" spans="2:3">
+    <row r="415" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B415" s="2"/>
       <c r="C415" s="2"/>
     </row>
-    <row r="416" spans="2:3">
+    <row r="416" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B416" s="2"/>
       <c r="C416" s="2"/>
     </row>
-    <row r="417" spans="1:4">
+    <row r="417" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A417" s="22"/>
       <c r="B417" s="17"/>
       <c r="C417" s="17"/>
       <c r="D417" s="18"/>
     </row>
-    <row r="418" spans="1:4">
+    <row r="418" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B418" s="2"/>
       <c r="C418" s="2"/>
     </row>
-    <row r="419" spans="1:4">
+    <row r="419" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B419" s="2"/>
       <c r="C419" s="2"/>
     </row>
-    <row r="420" spans="1:4">
+    <row r="420" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B420" s="2"/>
       <c r="C420" s="2"/>
     </row>
-    <row r="421" spans="1:4">
+    <row r="421" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B421" s="2"/>
       <c r="C421" s="2"/>
     </row>
-    <row r="422" spans="1:4">
+    <row r="422" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B422" s="2"/>
       <c r="C422" s="2"/>
     </row>
-    <row r="423" spans="1:4">
+    <row r="423" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B423" s="2"/>
       <c r="C423" s="2"/>
     </row>
-    <row r="424" spans="1:4">
+    <row r="424" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B424" s="2"/>
       <c r="C424" s="2"/>
     </row>
-    <row r="425" spans="1:4">
+    <row r="425" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B425" s="2"/>
       <c r="C425" s="2"/>
     </row>
-    <row r="426" spans="1:4">
+    <row r="426" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B426" s="2"/>
       <c r="C426" s="2"/>
     </row>
-    <row r="427" spans="1:4">
+    <row r="427" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B427" s="2"/>
       <c r="C427" s="2"/>
     </row>
-    <row r="428" spans="1:4">
+    <row r="428" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B428" s="2"/>
       <c r="C428" s="2"/>
     </row>
-    <row r="429" spans="1:4">
+    <row r="429" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B429" s="2"/>
       <c r="C429" s="2"/>
     </row>
-    <row r="430" spans="1:4">
+    <row r="430" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B430" s="2"/>
       <c r="C430" s="2"/>
     </row>
-    <row r="431" spans="1:4">
+    <row r="431" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B431" s="2"/>
       <c r="C431" s="2"/>
     </row>
-    <row r="432" spans="1:4">
+    <row r="432" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B432" s="2"/>
       <c r="C432" s="2"/>
     </row>
-    <row r="433" spans="1:4">
+    <row r="433" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B433" s="2"/>
       <c r="C433" s="2"/>
     </row>
-    <row r="434" spans="1:4">
+    <row r="434" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B434" s="2"/>
       <c r="C434" s="2"/>
     </row>
-    <row r="435" spans="1:4">
+    <row r="435" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A435" s="11"/>
       <c r="B435" s="17"/>
       <c r="C435" s="17"/>
       <c r="D435" s="18"/>
     </row>
-    <row r="436" spans="1:4">
+    <row r="436" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B436" s="2"/>
       <c r="C436" s="2"/>
     </row>
-    <row r="437" spans="1:4">
+    <row r="437" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B437" s="2"/>
       <c r="C437" s="2"/>
     </row>
-    <row r="438" spans="1:4">
+    <row r="438" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B438" s="2"/>
       <c r="C438" s="2"/>
     </row>
-    <row r="439" spans="1:4">
+    <row r="439" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B439" s="2"/>
       <c r="C439" s="2"/>
     </row>
-    <row r="440" spans="1:4">
+    <row r="440" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B440" s="2"/>
       <c r="C440" s="2"/>
     </row>
-    <row r="441" spans="1:4">
+    <row r="441" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B441" s="2"/>
       <c r="C441" s="2"/>
     </row>
-    <row r="442" spans="1:4">
+    <row r="442" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B442" s="2"/>
       <c r="C442" s="2"/>
     </row>
-    <row r="443" spans="1:4">
+    <row r="443" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B443" s="2"/>
       <c r="C443" s="2"/>
     </row>
-    <row r="444" spans="1:4">
+    <row r="444" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B444" s="2"/>
       <c r="C444" s="2"/>
     </row>
-    <row r="445" spans="1:4">
+    <row r="445" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B445" s="2"/>
       <c r="C445" s="2"/>
     </row>
-    <row r="446" spans="1:4">
+    <row r="446" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B446" s="2"/>
       <c r="C446" s="2"/>
     </row>
-    <row r="447" spans="1:4">
+    <row r="447" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B447" s="2"/>
       <c r="C447" s="2"/>
     </row>
-    <row r="448" spans="1:4">
+    <row r="448" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B448" s="2"/>
       <c r="C448" s="2"/>
     </row>
-    <row r="449" spans="1:3">
+    <row r="449" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B449" s="2"/>
       <c r="C449" s="2"/>
     </row>
-    <row r="450" spans="1:3">
+    <row r="450" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B450" s="2"/>
       <c r="C450" s="2"/>
     </row>
-    <row r="451" spans="1:3">
+    <row r="451" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B451" s="2"/>
       <c r="C451" s="2"/>
     </row>
-    <row r="452" spans="1:3">
+    <row r="452" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B452" s="2"/>
       <c r="C452" s="2"/>
     </row>
-    <row r="453" spans="1:3">
+    <row r="453" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A453" s="11"/>
       <c r="B453" s="17"/>
       <c r="C453" s="17"/>
     </row>
-    <row r="454" spans="1:3">
+    <row r="454" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B454" s="2"/>
       <c r="C454" s="2"/>
     </row>
-    <row r="455" spans="1:3">
+    <row r="455" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B455" s="2"/>
       <c r="C455" s="2"/>
     </row>
-    <row r="456" spans="1:3">
+    <row r="456" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B456" s="2"/>
       <c r="C456" s="2"/>
     </row>
-    <row r="457" spans="1:3">
+    <row r="457" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B457" s="2"/>
       <c r="C457" s="2"/>
     </row>
-    <row r="458" spans="1:3">
+    <row r="458" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B458" s="2"/>
       <c r="C458" s="2"/>
     </row>
-    <row r="459" spans="1:3">
+    <row r="459" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B459" s="2"/>
       <c r="C459" s="2"/>
     </row>
-    <row r="460" spans="1:3">
+    <row r="460" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B460" s="2"/>
       <c r="C460" s="2"/>
     </row>
-    <row r="461" spans="1:3">
+    <row r="461" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B461" s="2"/>
       <c r="C461" s="2"/>
     </row>
-    <row r="462" spans="1:3">
+    <row r="462" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B462" s="2"/>
       <c r="C462" s="2"/>
     </row>
-    <row r="463" spans="1:3">
+    <row r="463" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B463" s="2"/>
       <c r="C463" s="2"/>
     </row>
-    <row r="464" spans="1:3">
+    <row r="464" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B464" s="2"/>
       <c r="C464" s="2"/>
     </row>
-    <row r="465" spans="1:4">
+    <row r="465" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B465" s="2"/>
       <c r="C465" s="2"/>
     </row>
-    <row r="466" spans="1:4">
+    <row r="466" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B466" s="2"/>
       <c r="C466" s="2"/>
     </row>
-    <row r="467" spans="1:4">
+    <row r="467" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B467" s="2"/>
       <c r="C467" s="2"/>
     </row>
-    <row r="468" spans="1:4">
+    <row r="468" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B468" s="2"/>
       <c r="C468" s="2"/>
     </row>
-    <row r="469" spans="1:4">
+    <row r="469" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B469" s="2"/>
       <c r="C469" s="2"/>
     </row>
-    <row r="470" spans="1:4">
+    <row r="470" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B470" s="2"/>
       <c r="C470" s="2"/>
     </row>
-    <row r="471" spans="1:4">
+    <row r="471" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A471" s="12"/>
       <c r="B471" s="17"/>
       <c r="C471" s="17"/>
       <c r="D471" s="18"/>
     </row>
-    <row r="472" spans="1:4">
+    <row r="472" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B472" s="2"/>
       <c r="C472" s="2"/>
     </row>
-    <row r="473" spans="1:4">
+    <row r="473" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B473" s="2"/>
       <c r="C473" s="2"/>
     </row>
-    <row r="474" spans="1:4">
+    <row r="474" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B474" s="2"/>
       <c r="C474" s="2"/>
     </row>
-    <row r="475" spans="1:4">
+    <row r="475" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B475" s="2"/>
       <c r="C475" s="2"/>
     </row>
-    <row r="476" spans="1:4">
+    <row r="476" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B476" s="2"/>
       <c r="C476" s="2"/>
     </row>
-    <row r="477" spans="1:4">
+    <row r="477" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B477" s="2"/>
       <c r="C477" s="2"/>
     </row>
-    <row r="478" spans="1:4">
+    <row r="478" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B478" s="2"/>
       <c r="C478" s="2"/>
     </row>
-    <row r="479" spans="1:4">
+    <row r="479" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B479" s="2"/>
       <c r="C479" s="2"/>
     </row>
-    <row r="480" spans="1:4">
+    <row r="480" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B480" s="2"/>
       <c r="C480" s="2"/>
     </row>
-    <row r="481" spans="1:4">
+    <row r="481" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B481" s="2"/>
       <c r="C481" s="2"/>
     </row>
-    <row r="482" spans="1:4">
+    <row r="482" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B482" s="2"/>
       <c r="C482" s="2"/>
     </row>
-    <row r="483" spans="1:4">
+    <row r="483" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B483" s="2"/>
       <c r="C483" s="2"/>
     </row>
-    <row r="484" spans="1:4">
+    <row r="484" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B484" s="2"/>
       <c r="C484" s="2"/>
     </row>
-    <row r="485" spans="1:4">
+    <row r="485" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B485" s="2"/>
       <c r="C485" s="2"/>
     </row>
-    <row r="486" spans="1:4">
+    <row r="486" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B486" s="2"/>
       <c r="C486" s="2"/>
     </row>
-    <row r="487" spans="1:4">
+    <row r="487" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B487" s="2"/>
       <c r="C487" s="2"/>
     </row>
-    <row r="488" spans="1:4">
+    <row r="488" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B488" s="2"/>
       <c r="C488" s="2"/>
     </row>
-    <row r="489" spans="1:4">
+    <row r="489" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A489" s="22"/>
       <c r="B489" s="17"/>
       <c r="C489" s="17"/>
       <c r="D489" s="18"/>
     </row>
-    <row r="490" spans="1:4">
+    <row r="490" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B490" s="2"/>
       <c r="C490" s="2"/>
     </row>
-    <row r="491" spans="1:4">
+    <row r="491" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B491" s="2"/>
       <c r="C491" s="2"/>
     </row>
-    <row r="492" spans="1:4">
+    <row r="492" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B492" s="2"/>
       <c r="C492" s="2"/>
     </row>
-    <row r="493" spans="1:4">
+    <row r="493" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B493" s="2"/>
       <c r="C493" s="2"/>
     </row>
-    <row r="494" spans="1:4">
+    <row r="494" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B494" s="2"/>
       <c r="C494" s="2"/>
     </row>
-    <row r="495" spans="1:4">
+    <row r="495" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B495" s="2"/>
       <c r="C495" s="2"/>
     </row>
-    <row r="496" spans="1:4">
+    <row r="496" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B496" s="2"/>
       <c r="C496" s="2"/>
     </row>
-    <row r="497" spans="1:4">
+    <row r="497" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B497" s="2"/>
       <c r="C497" s="2"/>
     </row>
-    <row r="498" spans="1:4">
+    <row r="498" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B498" s="2"/>
       <c r="C498" s="2"/>
     </row>
-    <row r="499" spans="1:4">
+    <row r="499" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B499" s="2"/>
       <c r="C499" s="2"/>
     </row>
-    <row r="500" spans="1:4">
+    <row r="500" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B500" s="2"/>
       <c r="C500" s="2"/>
     </row>
-    <row r="501" spans="1:4">
+    <row r="501" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B501" s="2"/>
       <c r="C501" s="2"/>
     </row>
-    <row r="502" spans="1:4">
+    <row r="502" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B502" s="2"/>
       <c r="C502" s="2"/>
     </row>
-    <row r="503" spans="1:4">
+    <row r="503" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B503" s="2"/>
       <c r="C503" s="2"/>
     </row>
-    <row r="504" spans="1:4">
+    <row r="504" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B504" s="2"/>
       <c r="C504" s="2"/>
     </row>
-    <row r="505" spans="1:4">
+    <row r="505" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B505" s="2"/>
       <c r="C505" s="2"/>
     </row>
-    <row r="506" spans="1:4">
+    <row r="506" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B506" s="2"/>
       <c r="C506" s="2"/>
     </row>
-    <row r="507" spans="1:4">
+    <row r="507" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A507" s="22"/>
       <c r="B507" s="17"/>
       <c r="C507" s="17"/>
       <c r="D507" s="18"/>
     </row>
-    <row r="508" spans="1:4">
+    <row r="508" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B508" s="2"/>
       <c r="C508" s="2"/>
     </row>
-    <row r="509" spans="1:4">
+    <row r="509" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B509" s="2"/>
       <c r="C509" s="2"/>
     </row>
-    <row r="510" spans="1:4">
+    <row r="510" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B510" s="2"/>
       <c r="C510" s="2"/>
     </row>
-    <row r="511" spans="1:4">
+    <row r="511" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B511" s="2"/>
       <c r="C511" s="2"/>
     </row>
-    <row r="512" spans="1:4">
+    <row r="512" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B512" s="2"/>
       <c r="C512" s="2"/>
     </row>
-    <row r="513" spans="1:4">
+    <row r="513" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B513" s="2"/>
       <c r="C513" s="2"/>
     </row>
-    <row r="514" spans="1:4">
+    <row r="514" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B514" s="2"/>
       <c r="C514" s="2"/>
     </row>
-    <row r="515" spans="1:4">
+    <row r="515" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B515" s="2"/>
       <c r="C515" s="2"/>
     </row>
-    <row r="516" spans="1:4">
+    <row r="516" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B516" s="2"/>
       <c r="C516" s="2"/>
     </row>
-    <row r="517" spans="1:4">
+    <row r="517" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B517" s="2"/>
       <c r="C517" s="2"/>
     </row>
-    <row r="518" spans="1:4">
+    <row r="518" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B518" s="2"/>
       <c r="C518" s="2"/>
     </row>
-    <row r="519" spans="1:4">
+    <row r="519" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B519" s="2"/>
       <c r="C519" s="2"/>
     </row>
-    <row r="520" spans="1:4">
+    <row r="520" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B520" s="2"/>
       <c r="C520" s="2"/>
     </row>
-    <row r="521" spans="1:4">
+    <row r="521" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B521" s="2"/>
       <c r="C521" s="2"/>
     </row>
-    <row r="522" spans="1:4">
+    <row r="522" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B522" s="2"/>
       <c r="C522" s="2"/>
     </row>
-    <row r="523" spans="1:4">
+    <row r="523" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B523" s="2"/>
       <c r="C523" s="2"/>
     </row>
-    <row r="524" spans="1:4">
+    <row r="524" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B524" s="2"/>
       <c r="C524" s="2"/>
     </row>
-    <row r="525" spans="1:4">
+    <row r="525" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A525" s="24"/>
       <c r="B525" s="17"/>
       <c r="C525" s="17"/>
       <c r="D525" s="18"/>
     </row>
-    <row r="526" spans="1:4">
+    <row r="526" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B526" s="2"/>
       <c r="C526" s="2"/>
     </row>
-    <row r="527" spans="1:4">
+    <row r="527" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B527" s="2"/>
       <c r="C527" s="2"/>
     </row>
-    <row r="528" spans="1:4">
+    <row r="528" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B528" s="2"/>
       <c r="C528" s="2"/>
     </row>
-    <row r="529" spans="1:4">
+    <row r="529" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B529" s="2"/>
       <c r="C529" s="2"/>
     </row>
-    <row r="530" spans="1:4">
+    <row r="530" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B530" s="2"/>
       <c r="C530" s="2"/>
     </row>
-    <row r="531" spans="1:4">
+    <row r="531" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B531" s="2"/>
       <c r="C531" s="2"/>
     </row>
-    <row r="532" spans="1:4">
+    <row r="532" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B532" s="2"/>
       <c r="C532" s="2"/>
     </row>
-    <row r="533" spans="1:4">
+    <row r="533" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B533" s="2"/>
       <c r="C533" s="2"/>
     </row>
-    <row r="534" spans="1:4">
+    <row r="534" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B534" s="2"/>
       <c r="C534" s="2"/>
     </row>
-    <row r="535" spans="1:4">
+    <row r="535" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B535" s="2"/>
       <c r="C535" s="2"/>
     </row>
-    <row r="536" spans="1:4">
+    <row r="536" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B536" s="2"/>
       <c r="C536" s="2"/>
     </row>
-    <row r="537" spans="1:4">
+    <row r="537" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B537" s="2"/>
       <c r="C537" s="2"/>
     </row>
-    <row r="538" spans="1:4">
+    <row r="538" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B538" s="2"/>
       <c r="C538" s="2"/>
     </row>
-    <row r="539" spans="1:4">
+    <row r="539" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B539" s="2"/>
       <c r="C539" s="2"/>
     </row>
-    <row r="540" spans="1:4">
+    <row r="540" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B540" s="2"/>
       <c r="C540" s="2"/>
     </row>
-    <row r="541" spans="1:4">
+    <row r="541" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B541" s="2"/>
       <c r="C541" s="2"/>
     </row>
-    <row r="542" spans="1:4">
+    <row r="542" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B542" s="2"/>
       <c r="C542" s="2"/>
     </row>
-    <row r="543" spans="1:4">
+    <row r="543" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A543" s="22"/>
       <c r="B543" s="17"/>
       <c r="C543" s="17"/>
       <c r="D543" s="18"/>
     </row>
-    <row r="544" spans="1:4">
+    <row r="544" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B544" s="2"/>
       <c r="C544" s="2"/>
     </row>
-    <row r="545" spans="2:3">
+    <row r="545" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B545" s="2"/>
       <c r="C545" s="2"/>
     </row>
-    <row r="546" spans="2:3">
+    <row r="546" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B546" s="2"/>
       <c r="C546" s="2"/>
     </row>
-    <row r="547" spans="2:3">
+    <row r="547" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B547" s="2"/>
       <c r="C547" s="2"/>
     </row>
-    <row r="548" spans="2:3">
+    <row r="548" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B548" s="2"/>
       <c r="C548" s="2"/>
     </row>
-    <row r="549" spans="2:3">
+    <row r="549" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B549" s="2"/>
       <c r="C549" s="2"/>
     </row>
-    <row r="550" spans="2:3">
+    <row r="550" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B550" s="2"/>
       <c r="C550" s="2"/>
     </row>
-    <row r="551" spans="2:3">
+    <row r="551" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B551" s="2"/>
       <c r="C551" s="2"/>
     </row>
-    <row r="552" spans="2:3">
+    <row r="552" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B552" s="2"/>
       <c r="C552" s="2"/>
     </row>
-    <row r="553" spans="2:3">
+    <row r="553" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B553" s="2"/>
       <c r="C553" s="2"/>
     </row>
-    <row r="554" spans="2:3">
+    <row r="554" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B554" s="2"/>
       <c r="C554" s="2"/>
     </row>
-    <row r="555" spans="2:3">
+    <row r="555" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B555" s="2"/>
       <c r="C555" s="2"/>
     </row>
-    <row r="556" spans="2:3">
+    <row r="556" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B556" s="2"/>
       <c r="C556" s="2"/>
     </row>
-    <row r="557" spans="2:3">
+    <row r="557" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B557" s="2"/>
       <c r="C557" s="2"/>
     </row>
-    <row r="558" spans="2:3">
+    <row r="558" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B558" s="2"/>
       <c r="C558" s="2"/>
     </row>
-    <row r="559" spans="2:3">
+    <row r="559" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B559" s="2"/>
       <c r="C559" s="2"/>
     </row>
-    <row r="560" spans="2:3">
+    <row r="560" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B560" s="2"/>
       <c r="C560" s="2"/>
     </row>
-    <row r="561" spans="1:4">
+    <row r="561" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A561" s="22"/>
       <c r="B561" s="17"/>
       <c r="C561" s="17"/>
       <c r="D561" s="18"/>
     </row>
-    <row r="562" spans="1:4">
+    <row r="562" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B562" s="2"/>
       <c r="C562" s="2"/>
     </row>
-    <row r="563" spans="1:4">
+    <row r="563" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B563" s="2"/>
       <c r="C563" s="2"/>
     </row>
-    <row r="564" spans="1:4">
+    <row r="564" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B564" s="2"/>
       <c r="C564" s="2"/>
     </row>
-    <row r="565" spans="1:4">
+    <row r="565" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B565" s="2"/>
       <c r="C565" s="2"/>
     </row>
-    <row r="566" spans="1:4">
+    <row r="566" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B566" s="2"/>
       <c r="C566" s="2"/>
     </row>
-    <row r="567" spans="1:4">
+    <row r="567" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B567" s="2"/>
       <c r="C567" s="2"/>
     </row>
-    <row r="568" spans="1:4">
+    <row r="568" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B568" s="2"/>
       <c r="C568" s="2"/>
     </row>
-    <row r="569" spans="1:4">
+    <row r="569" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B569" s="2"/>
       <c r="C569" s="2"/>
     </row>
-    <row r="570" spans="1:4">
+    <row r="570" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B570" s="2"/>
       <c r="C570" s="2"/>
     </row>
-    <row r="571" spans="1:4">
+    <row r="571" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B571" s="2"/>
       <c r="C571" s="2"/>
     </row>
-    <row r="572" spans="1:4">
+    <row r="572" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B572" s="2"/>
       <c r="C572" s="2"/>
     </row>
-    <row r="573" spans="1:4">
+    <row r="573" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B573" s="2"/>
       <c r="C573" s="2"/>
     </row>
-    <row r="574" spans="1:4">
+    <row r="574" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B574" s="2"/>
       <c r="C574" s="2"/>
     </row>
-    <row r="575" spans="1:4">
+    <row r="575" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B575" s="2"/>
       <c r="C575" s="2"/>
     </row>
-    <row r="576" spans="1:4">
+    <row r="576" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B576" s="2"/>
       <c r="C576" s="2"/>
     </row>
-    <row r="577" spans="1:4">
+    <row r="577" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B577" s="2"/>
       <c r="C577" s="2"/>
     </row>
-    <row r="578" spans="1:4">
+    <row r="578" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B578" s="2"/>
       <c r="C578" s="2"/>
     </row>
-    <row r="579" spans="1:4">
+    <row r="579" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A579" s="21"/>
       <c r="B579" s="17"/>
       <c r="C579" s="17"/>
       <c r="D579" s="18"/>
     </row>
-    <row r="580" spans="1:4">
+    <row r="580" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B580" s="2"/>
       <c r="C580" s="2"/>
     </row>
-    <row r="581" spans="1:4">
+    <row r="581" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B581" s="2"/>
       <c r="C581" s="2"/>
     </row>
-    <row r="582" spans="1:4">
+    <row r="582" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B582" s="2"/>
       <c r="C582" s="2"/>
     </row>
-    <row r="583" spans="1:4">
+    <row r="583" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B583" s="2"/>
       <c r="C583" s="2"/>
     </row>
-    <row r="584" spans="1:4">
+    <row r="584" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B584" s="2"/>
       <c r="C584" s="2"/>
     </row>
-    <row r="585" spans="1:4">
+    <row r="585" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B585" s="2"/>
       <c r="C585" s="2"/>
     </row>
-    <row r="586" spans="1:4">
+    <row r="586" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B586" s="2"/>
       <c r="C586" s="2"/>
     </row>
-    <row r="587" spans="1:4">
+    <row r="587" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B587" s="2"/>
       <c r="C587" s="2"/>
     </row>
-    <row r="588" spans="1:4">
+    <row r="588" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B588" s="2"/>
       <c r="C588" s="2"/>
     </row>
-    <row r="589" spans="1:4">
+    <row r="589" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B589" s="2"/>
       <c r="C589" s="2"/>
     </row>
-    <row r="590" spans="1:4">
+    <row r="590" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B590" s="2"/>
       <c r="C590" s="2"/>
     </row>
-    <row r="591" spans="1:4">
+    <row r="591" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B591" s="2"/>
       <c r="C591" s="2"/>
     </row>
-    <row r="592" spans="1:4">
+    <row r="592" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B592" s="2"/>
       <c r="C592" s="2"/>
     </row>
-    <row r="593" spans="1:4">
+    <row r="593" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B593" s="2"/>
       <c r="C593" s="2"/>
     </row>
-    <row r="594" spans="1:4">
+    <row r="594" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B594" s="2"/>
       <c r="C594" s="2"/>
     </row>
-    <row r="595" spans="1:4">
+    <row r="595" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B595" s="2"/>
       <c r="C595" s="2"/>
     </row>
-    <row r="596" spans="1:4">
+    <row r="596" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B596" s="2"/>
       <c r="C596" s="2"/>
     </row>
-    <row r="597" spans="1:4">
+    <row r="597" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A597" s="23"/>
       <c r="B597" s="17"/>
       <c r="C597" s="17"/>
       <c r="D597" s="18"/>
     </row>
-    <row r="598" spans="1:4">
+    <row r="598" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B598" s="2"/>
       <c r="C598" s="2"/>
     </row>
-    <row r="599" spans="1:4">
+    <row r="599" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B599" s="2"/>
       <c r="C599" s="2"/>
     </row>
-    <row r="600" spans="1:4">
+    <row r="600" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B600" s="2"/>
       <c r="C600" s="2"/>
     </row>
-    <row r="601" spans="1:4">
+    <row r="601" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B601" s="2"/>
       <c r="C601" s="2"/>
     </row>
-    <row r="602" spans="1:4">
+    <row r="602" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B602" s="2"/>
       <c r="C602" s="2"/>
     </row>
-    <row r="603" spans="1:4">
+    <row r="603" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B603" s="2"/>
       <c r="C603" s="2"/>
     </row>
-    <row r="604" spans="1:4">
+    <row r="604" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B604" s="2"/>
       <c r="C604" s="2"/>
     </row>
-    <row r="605" spans="1:4">
+    <row r="605" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B605" s="2"/>
       <c r="C605" s="2"/>
     </row>
-    <row r="606" spans="1:4">
+    <row r="606" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B606" s="2"/>
       <c r="C606" s="2"/>
     </row>
-    <row r="607" spans="1:4">
+    <row r="607" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B607" s="2"/>
       <c r="C607" s="2"/>
     </row>
-    <row r="608" spans="1:4">
+    <row r="608" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B608" s="2"/>
       <c r="C608" s="2"/>
     </row>
-    <row r="609" spans="1:4">
+    <row r="609" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B609" s="2"/>
       <c r="C609" s="2"/>
     </row>
-    <row r="610" spans="1:4">
+    <row r="610" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B610" s="2"/>
       <c r="C610" s="2"/>
     </row>
-    <row r="611" spans="1:4">
+    <row r="611" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B611" s="2"/>
       <c r="C611" s="2"/>
     </row>
-    <row r="612" spans="1:4">
+    <row r="612" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B612" s="2"/>
       <c r="C612" s="2"/>
     </row>
-    <row r="613" spans="1:4">
+    <row r="613" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B613" s="2"/>
       <c r="C613" s="2"/>
     </row>
-    <row r="614" spans="1:4">
+    <row r="614" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B614" s="2"/>
       <c r="C614" s="2"/>
     </row>
-    <row r="615" spans="1:4">
+    <row r="615" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A615" s="23"/>
       <c r="B615" s="17"/>
       <c r="C615" s="17"/>
       <c r="D615" s="18"/>
     </row>
-    <row r="616" spans="1:4">
+    <row r="616" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B616" s="2"/>
       <c r="C616" s="2"/>
     </row>
-    <row r="617" spans="1:4">
+    <row r="617" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B617" s="2"/>
       <c r="C617" s="2"/>
     </row>
-    <row r="618" spans="1:4">
+    <row r="618" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B618" s="2"/>
       <c r="C618" s="2"/>
     </row>
-    <row r="619" spans="1:4">
+    <row r="619" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B619" s="2"/>
       <c r="C619" s="2"/>
     </row>
-    <row r="620" spans="1:4">
+    <row r="620" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B620" s="2"/>
       <c r="C620" s="2"/>
     </row>
-    <row r="621" spans="1:4">
+    <row r="621" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B621" s="2"/>
       <c r="C621" s="2"/>
     </row>
-    <row r="622" spans="1:4">
+    <row r="622" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B622" s="2"/>
       <c r="C622" s="2"/>
     </row>
-    <row r="623" spans="1:4">
+    <row r="623" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B623" s="2"/>
       <c r="C623" s="2"/>
     </row>
-    <row r="624" spans="1:4">
+    <row r="624" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B624" s="2"/>
       <c r="C624" s="2"/>
     </row>
-    <row r="625" spans="1:4">
+    <row r="625" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B625" s="2"/>
       <c r="C625" s="2"/>
     </row>
-    <row r="626" spans="1:4">
+    <row r="626" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B626" s="2"/>
       <c r="C626" s="2"/>
     </row>
-    <row r="627" spans="1:4">
+    <row r="627" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B627" s="2"/>
       <c r="C627" s="2"/>
     </row>
-    <row r="628" spans="1:4">
+    <row r="628" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B628" s="2"/>
       <c r="C628" s="2"/>
     </row>
-    <row r="629" spans="1:4">
+    <row r="629" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B629" s="2"/>
       <c r="C629" s="2"/>
     </row>
-    <row r="630" spans="1:4">
+    <row r="630" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B630" s="2"/>
       <c r="C630" s="2"/>
     </row>
-    <row r="631" spans="1:4">
+    <row r="631" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B631" s="2"/>
       <c r="C631" s="2"/>
     </row>
-    <row r="632" spans="1:4">
+    <row r="632" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B632" s="2"/>
       <c r="C632" s="2"/>
     </row>
-    <row r="633" spans="1:4">
+    <row r="633" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A633" s="23"/>
       <c r="B633" s="17"/>
       <c r="C633" s="17"/>
       <c r="D633" s="18"/>
     </row>
-    <row r="634" spans="1:4">
+    <row r="634" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B634" s="2"/>
       <c r="C634" s="2"/>
     </row>
-    <row r="635" spans="1:4">
+    <row r="635" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B635" s="2"/>
       <c r="C635" s="2"/>
     </row>
-    <row r="636" spans="1:4">
+    <row r="636" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B636" s="2"/>
       <c r="C636" s="2"/>
     </row>
-    <row r="637" spans="1:4">
+    <row r="637" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B637" s="2"/>
       <c r="C637" s="2"/>
     </row>
-    <row r="638" spans="1:4">
+    <row r="638" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B638" s="2"/>
       <c r="C638" s="2"/>
     </row>
-    <row r="639" spans="1:4">
+    <row r="639" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B639" s="2"/>
       <c r="C639" s="2"/>
     </row>
-    <row r="640" spans="1:4">
+    <row r="640" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B640" s="2"/>
       <c r="C640" s="2"/>
     </row>
-    <row r="641" spans="1:4">
+    <row r="641" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B641" s="2"/>
       <c r="C641" s="2"/>
     </row>
-    <row r="642" spans="1:4">
+    <row r="642" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B642" s="2"/>
       <c r="C642" s="2"/>
     </row>
-    <row r="643" spans="1:4">
+    <row r="643" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B643" s="2"/>
       <c r="C643" s="2"/>
     </row>
-    <row r="644" spans="1:4">
+    <row r="644" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B644" s="2"/>
       <c r="C644" s="2"/>
     </row>
-    <row r="645" spans="1:4">
+    <row r="645" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B645" s="2"/>
       <c r="C645" s="2"/>
     </row>
-    <row r="646" spans="1:4">
+    <row r="646" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B646" s="2"/>
       <c r="C646" s="2"/>
     </row>
-    <row r="647" spans="1:4">
+    <row r="647" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B647" s="2"/>
       <c r="C647" s="2"/>
     </row>
-    <row r="648" spans="1:4">
+    <row r="648" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B648" s="2"/>
       <c r="C648" s="2"/>
     </row>
-    <row r="649" spans="1:4">
+    <row r="649" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B649" s="2"/>
       <c r="C649" s="2"/>
     </row>
-    <row r="650" spans="1:4">
+    <row r="650" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B650" s="2"/>
       <c r="C650" s="2"/>
     </row>
-    <row r="651" spans="1:4">
+    <row r="651" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A651" s="22"/>
       <c r="B651" s="17"/>
       <c r="C651" s="17"/>
       <c r="D651" s="18"/>
     </row>
-    <row r="652" spans="1:4">
+    <row r="652" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B652" s="2"/>
       <c r="C652" s="2"/>
     </row>
-    <row r="653" spans="1:4">
+    <row r="653" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B653" s="2"/>
       <c r="C653" s="2"/>
     </row>
-    <row r="654" spans="1:4">
+    <row r="654" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B654" s="2"/>
       <c r="C654" s="2"/>
     </row>
-    <row r="655" spans="1:4">
+    <row r="655" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B655" s="2"/>
       <c r="C655" s="2"/>
     </row>
-    <row r="656" spans="1:4">
+    <row r="656" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B656" s="2"/>
       <c r="C656" s="2"/>
     </row>
-    <row r="657" spans="1:4">
+    <row r="657" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B657" s="2"/>
       <c r="C657" s="2"/>
     </row>
-    <row r="658" spans="1:4">
+    <row r="658" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B658" s="2"/>
       <c r="C658" s="2"/>
     </row>
-    <row r="659" spans="1:4">
+    <row r="659" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B659" s="2"/>
       <c r="C659" s="2"/>
     </row>
-    <row r="660" spans="1:4">
+    <row r="660" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B660" s="2"/>
       <c r="C660" s="2"/>
     </row>
-    <row r="661" spans="1:4">
+    <row r="661" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B661" s="2"/>
       <c r="C661" s="2"/>
     </row>
-    <row r="662" spans="1:4">
+    <row r="662" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B662" s="2"/>
       <c r="C662" s="2"/>
     </row>
-    <row r="663" spans="1:4">
+    <row r="663" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B663" s="2"/>
       <c r="C663" s="2"/>
     </row>
-    <row r="664" spans="1:4">
+    <row r="664" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B664" s="2"/>
       <c r="C664" s="2"/>
     </row>
-    <row r="665" spans="1:4">
+    <row r="665" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B665" s="2"/>
       <c r="C665" s="2"/>
     </row>
-    <row r="666" spans="1:4">
+    <row r="666" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B666" s="2"/>
       <c r="C666" s="2"/>
     </row>
-    <row r="667" spans="1:4">
+    <row r="667" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B667" s="2"/>
       <c r="C667" s="2"/>
     </row>
-    <row r="668" spans="1:4">
+    <row r="668" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B668" s="2"/>
       <c r="C668" s="2"/>
     </row>
-    <row r="669" spans="1:4">
+    <row r="669" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A669" s="21"/>
       <c r="B669" s="17"/>
       <c r="C669" s="17"/>
       <c r="D669" s="18"/>
     </row>
-    <row r="670" spans="1:4">
+    <row r="670" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B670" s="2"/>
       <c r="C670" s="2"/>
     </row>
-    <row r="671" spans="1:4">
+    <row r="671" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B671" s="2"/>
       <c r="C671" s="2"/>
     </row>
-    <row r="672" spans="1:4">
+    <row r="672" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B672" s="2"/>
       <c r="C672" s="2"/>
     </row>
-    <row r="673" spans="2:3">
+    <row r="673" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B673" s="2"/>
       <c r="C673" s="2"/>
     </row>
-    <row r="674" spans="2:3">
+    <row r="674" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B674" s="2"/>
       <c r="C674" s="2"/>
     </row>
-    <row r="675" spans="2:3">
+    <row r="675" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B675" s="2"/>
       <c r="C675" s="2"/>
     </row>
-    <row r="676" spans="2:3">
+    <row r="676" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B676" s="2"/>
       <c r="C676" s="2"/>
     </row>
-    <row r="677" spans="2:3">
+    <row r="677" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B677" s="2"/>
       <c r="C677" s="2"/>
     </row>
-    <row r="678" spans="2:3">
+    <row r="678" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B678" s="2"/>
       <c r="C678" s="2"/>
     </row>
-    <row r="679" spans="2:3">
+    <row r="679" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B679" s="2"/>
       <c r="C679" s="2"/>
     </row>
-    <row r="680" spans="2:3">
+    <row r="680" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B680" s="2"/>
       <c r="C680" s="2"/>
     </row>
-    <row r="681" spans="2:3">
+    <row r="681" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B681" s="2"/>
       <c r="C681" s="2"/>
     </row>
-    <row r="682" spans="2:3">
+    <row r="682" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B682" s="2"/>
       <c r="C682" s="2"/>
     </row>
-    <row r="683" spans="2:3">
+    <row r="683" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B683" s="2"/>
       <c r="C683" s="2"/>
     </row>
-    <row r="684" spans="2:3">
+    <row r="684" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B684" s="2"/>
       <c r="C684" s="2"/>
     </row>
-    <row r="685" spans="2:3">
+    <row r="685" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B685" s="2"/>
       <c r="C685" s="2"/>
     </row>
-    <row r="686" spans="2:3">
+    <row r="686" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B686" s="2"/>
       <c r="C686" s="2"/>
     </row>
@@ -5314,14 +5382,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.83203125" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
@@ -5330,7 +5398,7 @@
     <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>68</v>
       </c>
@@ -5347,7 +5415,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -5376,21 +5444,21 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.83203125" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>32</v>
       </c>
@@ -5401,7 +5469,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>85</v>
       </c>
@@ -5412,7 +5480,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>85</v>
       </c>

</xml_diff>